<commit_message>
Added html etc for the 3 missing crafting skills.
</commit_message>
<xml_diff>
--- a/Charsheet_RMSS_categoriesandskills.xlsx
+++ b/Charsheet_RMSS_categoriesandskills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="27375" windowHeight="11970" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="27375" windowHeight="11970" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Calculations" sheetId="7" r:id="rId1"/>
@@ -12739,7 +12739,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -12749,6 +12749,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -12765,12 +12771,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -15195,9 +15202,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O310"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18998,7 +19005,7 @@
       <c r="A87" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" s="5" t="s">
         <v>339</v>
       </c>
       <c r="C87" t="s">
@@ -19086,7 +19093,7 @@
       <c r="A89" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" s="5" t="s">
         <v>340</v>
       </c>
       <c r="C89" t="s">
@@ -19306,7 +19313,7 @@
       <c r="A94" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" s="5" t="s">
         <v>341</v>
       </c>
       <c r="C94" t="s">
@@ -28852,6 +28859,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -33969,7 +33977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DP24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BS1" workbookViewId="0">
+    <sheetView topLeftCell="BS1" workbookViewId="0">
       <selection activeCell="DO23" sqref="DO23"/>
     </sheetView>
   </sheetViews>
@@ -42058,7 +42066,7 @@
         <v>4130</v>
       </c>
       <c r="Y3" t="str">
-        <f>CONCATENATE(,O3,P3,Q3,R3,S3,T3,U3,V3,W3,X3)</f>
+        <f t="shared" ref="Y3:Y8" si="0">CONCATENATE(,O3,P3,Q3,R3,S3,T3,U3,V3,W3,X3)</f>
         <v>D3,": ",E3,", ",f3,": ",g3,", ",h3,": ",i3,", ",j3,": ",k3,", ",l3,": ",m3,", ",n3,": ",o3,", ",p3,": ",q3,", ",r3,": ",s3,", ",t3,": ",u3,", ",v3,": ",w3,", ",</v>
       </c>
     </row>
@@ -42082,7 +42090,7 @@
         <v>4120</v>
       </c>
       <c r="J4" t="str">
-        <f t="shared" ref="J4:J59" si="0">CONCATENATE(B4,C4,D4,E4,F4,G4,H4,I4)</f>
+        <f t="shared" ref="J4:J59" si="1">CONCATENATE(B4,C4,D4,E4,F4,G4,H4,I4)</f>
         <v>f3,": ",g3,", ",</v>
       </c>
       <c r="M4" t="s">
@@ -42119,7 +42127,7 @@
         <v>4140</v>
       </c>
       <c r="Y4" t="str">
-        <f t="shared" ref="Y4:Y8" si="1">CONCATENATE(,O4,P4,Q4,R4,S4,T4,U4,V4,W4,X4)</f>
+        <f t="shared" si="0"/>
         <v>x3,": ",y3,", ",z3,": ",aa3,", ",ab3,": ",ac3,", ",ad3,": ",ae3,", ",af3,": ",ag3,", ",ah3,": ",ai3,", ",aj3,": ",ak3,", ",al3,": ",am3,", ",an3,": ",ao3,", ",ap3,": ",aq3,", ",</v>
       </c>
     </row>
@@ -42143,7 +42151,7 @@
         <v>4120</v>
       </c>
       <c r="J5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>h3,": ",i3,", ",</v>
       </c>
       <c r="M5" t="s">
@@ -42180,7 +42188,7 @@
         <v>4150</v>
       </c>
       <c r="Y5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>ar3,": ",as3,", ",at3,": ",au3,", ",av3,": ",aw3,", ",ax3,": ",ay3,", ",az3,": ",ba3,", ",bb3,": ",bc3,", ",bd3,": ",be3,", ",bf3,": ",bg3,", ",bh3,": ",bi3,", ",bj3,": ",bk3,", ",</v>
       </c>
     </row>
@@ -42204,7 +42212,7 @@
         <v>4120</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>j3,": ",k3,", ",</v>
       </c>
       <c r="M6" t="s">
@@ -42241,7 +42249,7 @@
         <v>4160</v>
       </c>
       <c r="Y6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>bl3,": ",bm3,", ",bn3,": ",bo3,", ",bp3,": ",bq3,", ",br3,": ",bs3,", ",bt3,": ",bu3,", ",bv3,": ",bw3,", ",bx3,": ",by3,", ",bz3,": ",ca3,", ",cb3,": ",cc3,", ",cd3,": ",ce3,", ",</v>
       </c>
     </row>
@@ -42265,7 +42273,7 @@
         <v>4120</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>l3,": ",m3,", ",</v>
       </c>
       <c r="M7" t="s">
@@ -42302,7 +42310,7 @@
         <v>4170</v>
       </c>
       <c r="Y7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>cf3,": ",cg3,", ",ch3,": ",ci3,", ",cj3,": ",ck3,", ",cl3,": ",cm3,", ",cn3,": ",co3,", ",cp3,": ",cq3,", ",cr3,": ",cs3,", ",ct3,": ",cu3,", ",cv3,": ",cw3,", ",cx3,": ",cy3,", ",</v>
       </c>
     </row>
@@ -42326,7 +42334,7 @@
         <v>4120</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>n3,": ",o3,", ",</v>
       </c>
       <c r="M8" t="s">
@@ -42354,7 +42362,7 @@
         <v>4177</v>
       </c>
       <c r="Y8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>cz3,": ",da3,", ",db3,": ",dc3,", ",dd3,": ",de3,", ",df3,": ",dg3,", ",dh3,": ",di3,", ",dj3,": ",dk3,", ",dl3,": ",dm3</v>
       </c>
     </row>
@@ -42378,7 +42386,7 @@
         <v>4120</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>p3,": ",q3,", ",</v>
       </c>
       <c r="M9" t="s">
@@ -42405,7 +42413,7 @@
         <v>4120</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>r3,": ",s3,", ",</v>
       </c>
       <c r="M10" t="s">
@@ -42432,7 +42440,7 @@
         <v>4120</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>t3,": ",u3,", ",</v>
       </c>
       <c r="M11" t="s">
@@ -42462,7 +42470,7 @@
         <v>4120</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>v3,": ",w3,", ",</v>
       </c>
       <c r="M12" t="s">
@@ -42492,7 +42500,7 @@
         <v>4120</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>x3,": ",y3,", ",</v>
       </c>
       <c r="M13" t="s">
@@ -42525,7 +42533,7 @@
         <v>4120</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>z3,": ",aa3,", ",</v>
       </c>
       <c r="M14" t="s">
@@ -42561,7 +42569,7 @@
         <v>4120</v>
       </c>
       <c r="J15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ab3,": ",ac3,", ",</v>
       </c>
       <c r="M15" t="s">
@@ -42597,7 +42605,7 @@
         <v>4120</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ad3,": ",ae3,", ",</v>
       </c>
       <c r="M16" t="s">
@@ -42633,7 +42641,7 @@
         <v>4120</v>
       </c>
       <c r="J17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>af3,": ",ag3,", ",</v>
       </c>
       <c r="M17" t="s">
@@ -42666,7 +42674,7 @@
         <v>4120</v>
       </c>
       <c r="J18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ah3,": ",ai3,", ",</v>
       </c>
       <c r="M18" t="s">
@@ -42699,7 +42707,7 @@
         <v>4120</v>
       </c>
       <c r="J19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>aj3,": ",ak3,", ",</v>
       </c>
       <c r="M19" t="s">
@@ -42754,7 +42762,7 @@
         <v>4120</v>
       </c>
       <c r="J20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>al3,": ",am3,", ",</v>
       </c>
       <c r="M20" t="s">
@@ -42787,7 +42795,7 @@
         <v>4120</v>
       </c>
       <c r="J21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>an3,": ",ao3,", ",</v>
       </c>
       <c r="M21" t="s">
@@ -42820,7 +42828,7 @@
         <v>4120</v>
       </c>
       <c r="J22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ap3,": ",aq3,", ",</v>
       </c>
       <c r="M22" t="s">
@@ -42856,7 +42864,7 @@
         <v>4120</v>
       </c>
       <c r="J23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ar3,": ",as3,", ",</v>
       </c>
       <c r="M23" t="s">
@@ -42889,7 +42897,7 @@
         <v>4120</v>
       </c>
       <c r="J24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>at3,": ",au3,", ",</v>
       </c>
       <c r="M24" t="s">
@@ -42922,7 +42930,7 @@
         <v>4120</v>
       </c>
       <c r="J25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>av3,": ",aw3,", ",</v>
       </c>
       <c r="M25" t="s">
@@ -42955,7 +42963,7 @@
         <v>4120</v>
       </c>
       <c r="J26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ax3,": ",ay3,", ",</v>
       </c>
       <c r="M26" t="s">
@@ -42988,7 +42996,7 @@
         <v>4120</v>
       </c>
       <c r="J27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>az3,": ",ba3,", ",</v>
       </c>
       <c r="M27" t="s">
@@ -43021,7 +43029,7 @@
         <v>4120</v>
       </c>
       <c r="J28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>bb3,": ",bc3,", ",</v>
       </c>
       <c r="M28" t="s">
@@ -43054,7 +43062,7 @@
         <v>4120</v>
       </c>
       <c r="J29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>bd3,": ",be3,", ",</v>
       </c>
       <c r="M29" t="s">
@@ -43087,7 +43095,7 @@
         <v>4120</v>
       </c>
       <c r="J30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>bf3,": ",bg3,", ",</v>
       </c>
       <c r="M30" t="s">
@@ -43120,7 +43128,7 @@
         <v>4120</v>
       </c>
       <c r="J31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>bh3,": ",bi3,", ",</v>
       </c>
       <c r="M31" t="s">
@@ -43153,7 +43161,7 @@
         <v>4120</v>
       </c>
       <c r="J32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>bj3,": ",bk3,", ",</v>
       </c>
       <c r="M32" t="s">
@@ -43186,7 +43194,7 @@
         <v>4120</v>
       </c>
       <c r="J33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>bl3,": ",bm3,", ",</v>
       </c>
       <c r="M33" t="s">
@@ -43219,7 +43227,7 @@
         <v>4120</v>
       </c>
       <c r="J34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>bn3,": ",bo3,", ",</v>
       </c>
       <c r="M34" t="s">
@@ -43252,7 +43260,7 @@
         <v>4120</v>
       </c>
       <c r="J35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>bp3,": ",bq3,", ",</v>
       </c>
       <c r="M35" t="s">
@@ -43285,7 +43293,7 @@
         <v>4120</v>
       </c>
       <c r="J36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>br3,": ",bs3,", ",</v>
       </c>
       <c r="M36" t="s">
@@ -43318,7 +43326,7 @@
         <v>4120</v>
       </c>
       <c r="J37" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>bt3,": ",bu3,", ",</v>
       </c>
       <c r="M37" t="s">
@@ -43351,7 +43359,7 @@
         <v>4120</v>
       </c>
       <c r="J38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>bv3,": ",bw3,", ",</v>
       </c>
       <c r="M38" t="s">
@@ -43384,7 +43392,7 @@
         <v>4120</v>
       </c>
       <c r="J39" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>bx3,": ",by3,", ",</v>
       </c>
       <c r="M39" t="s">
@@ -43417,7 +43425,7 @@
         <v>4120</v>
       </c>
       <c r="J40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>bz3,": ",ca3,", ",</v>
       </c>
       <c r="M40" t="s">
@@ -43450,7 +43458,7 @@
         <v>4120</v>
       </c>
       <c r="J41" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>cb3,": ",cc3,", ",</v>
       </c>
       <c r="M41" t="s">
@@ -43483,7 +43491,7 @@
         <v>4120</v>
       </c>
       <c r="J42" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>cd3,": ",ce3,", ",</v>
       </c>
       <c r="M42" t="s">
@@ -43516,7 +43524,7 @@
         <v>4120</v>
       </c>
       <c r="J43" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>cf3,": ",cg3,", ",</v>
       </c>
       <c r="M43" t="s">
@@ -43549,7 +43557,7 @@
         <v>4120</v>
       </c>
       <c r="J44" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ch3,": ",ci3,", ",</v>
       </c>
       <c r="M44" t="s">
@@ -43582,7 +43590,7 @@
         <v>4120</v>
       </c>
       <c r="J45" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>cj3,": ",ck3,", ",</v>
       </c>
       <c r="M45" t="s">
@@ -43615,7 +43623,7 @@
         <v>4120</v>
       </c>
       <c r="J46" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>cl3,": ",cm3,", ",</v>
       </c>
       <c r="M46" t="s">
@@ -43648,7 +43656,7 @@
         <v>4120</v>
       </c>
       <c r="J47" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>cn3,": ",co3,", ",</v>
       </c>
       <c r="M47" t="s">
@@ -43681,7 +43689,7 @@
         <v>4120</v>
       </c>
       <c r="J48" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>cp3,": ",cq3,", ",</v>
       </c>
       <c r="M48" t="s">
@@ -43714,7 +43722,7 @@
         <v>4120</v>
       </c>
       <c r="J49" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>cr3,": ",cs3,", ",</v>
       </c>
       <c r="M49" t="s">
@@ -43747,7 +43755,7 @@
         <v>4120</v>
       </c>
       <c r="J50" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ct3,": ",cu3,", ",</v>
       </c>
       <c r="M50" t="s">
@@ -43780,7 +43788,7 @@
         <v>4120</v>
       </c>
       <c r="J51" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>cv3,": ",cw3,", ",</v>
       </c>
       <c r="M51" t="s">
@@ -43813,7 +43821,7 @@
         <v>4120</v>
       </c>
       <c r="J52" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>cx3,": ",cy3,", ",</v>
       </c>
       <c r="M52" t="s">
@@ -43846,7 +43854,7 @@
         <v>4120</v>
       </c>
       <c r="J53" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>cz3,": ",da3,", ",</v>
       </c>
       <c r="M53" t="s">
@@ -43879,7 +43887,7 @@
         <v>4120</v>
       </c>
       <c r="J54" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>db3,": ",dc3,", ",</v>
       </c>
       <c r="M54" t="s">
@@ -43912,7 +43920,7 @@
         <v>4120</v>
       </c>
       <c r="J55" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>dd3,": ",de3,", ",</v>
       </c>
       <c r="M55" t="s">
@@ -43945,7 +43953,7 @@
         <v>4120</v>
       </c>
       <c r="J56" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>df3,": ",dg3,", ",</v>
       </c>
       <c r="M56" t="s">
@@ -43978,7 +43986,7 @@
         <v>4120</v>
       </c>
       <c r="J57" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>dh3,": ",di3,", ",</v>
       </c>
       <c r="M57" t="s">
@@ -44011,7 +44019,7 @@
         <v>4120</v>
       </c>
       <c r="J58" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>dj3,": ",dk3,", ",</v>
       </c>
       <c r="M58" t="s">
@@ -44041,7 +44049,7 @@
         <v>3</v>
       </c>
       <c r="J59" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>dl3,": ",dm3</v>
       </c>
       <c r="M59" t="s">

</xml_diff>